<commit_message>
update excel column names
</commit_message>
<xml_diff>
--- a/Data/Burundi final test v2.xlsx
+++ b/Data/Burundi final test v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Documents\GitHub\IRP-framework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AC8B5C-38F0-4BAC-93A7-582A5C063AFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D573A8-75F0-4751-9384-5678704B5131}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
+    <workbookView xWindow="435" yWindow="1132" windowWidth="21608" windowHeight="10516" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Schools" sheetId="1" r:id="rId1"/>
@@ -132,12 +132,6 @@
     <t>Total Sum of Commodities</t>
   </si>
   <si>
-    <t>Consumption per day in mt</t>
-  </si>
-  <si>
-    <t>Consumption per week in mt</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>CD107-69U</t>
+  </si>
+  <si>
+    <t>Consumption per day in MT</t>
+  </si>
+  <si>
+    <t>Consumption per week in MT</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1058,8 @@
     <tableColumn id="1" xr3:uid="{E5C5CD31-DB14-4BCA-9F11-3AA7A7551D2B}" name="Name_ID" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{EB335BE7-11E3-434A-B317-30C0F850D50E}" name="Total Sum of Beneficiaries" dataDxfId="27"/>
     <tableColumn id="4" xr3:uid="{548C3917-F847-4593-A558-D428505FFBD5}" name="Total Sum of Commodities" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{FE888112-53D5-4BA1-A73D-44D889EF4C4D}" name="Consumption per day in mt" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{16626E44-7904-4057-88C7-E83A60A6E39B}" name="Consumption per week in mt" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{FE888112-53D5-4BA1-A73D-44D889EF4C4D}" name="Consumption per day in MT" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{16626E44-7904-4057-88C7-E83A60A6E39B}" name="Consumption per week in MT" dataDxfId="24"/>
     <tableColumn id="7" xr3:uid="{BCB38217-DC5E-4A6B-90D0-4ED4225CA0CB}" name="Latitude" dataDxfId="23"/>
     <tableColumn id="8" xr3:uid="{26DFB5ED-C9CB-4B62-A8A1-67C23CE6A976}" name="Longitude" dataDxfId="22"/>
     <tableColumn id="10" xr3:uid="{AAB748E8-3709-4A83-AC4C-F11F31AEC3F8}" name="Capacity" dataDxfId="21"/>
@@ -1400,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65252ADD-2539-421B-8440-8530B4AE7D99}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1425,33 +1425,33 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>409</v>
@@ -1486,7 +1486,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>556</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>664</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>866</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>635</v>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>1168</v>
@@ -1661,7 +1661,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>590</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>847</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>848</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>708</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>903</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>635</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
         <v>1160</v>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>548</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <v>551</v>
@@ -1989,7 +1989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5307C4E-D51E-4E16-960B-CB790613AD8F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2004,27 +2004,27 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1">
         <v>-3.36</v>
@@ -2047,7 +2047,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1">
         <v>-2.911</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1">
         <v>-3.4279999999999999</v>
@@ -2114,33 +2114,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
       <c r="E2" s="9">
         <v>18</v>
@@ -2148,16 +2148,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E3" s="9">
         <v>18</v>
@@ -2165,16 +2165,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="9">
         <v>8</v>
@@ -2182,16 +2182,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="9">
         <v>8</v>
@@ -2199,16 +2199,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="9">
         <v>8</v>
@@ -2216,13 +2216,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2233,16 +2233,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
         <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
       </c>
       <c r="E8" s="9">
         <v>1.5</v>
@@ -2250,13 +2250,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2267,16 +2267,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" s="9">
         <v>18</v>
@@ -2284,16 +2284,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="9">
         <v>8</v>
@@ -2301,13 +2301,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2318,13 +2318,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -2335,13 +2335,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2352,13 +2352,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2386,13 +2386,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2403,16 +2403,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E18" s="9">
         <v>1.5</v>
@@ -2420,16 +2420,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19" s="9">
         <v>1.5</v>
@@ -2437,16 +2437,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E20" s="9">
         <v>18</v>
@@ -2454,16 +2454,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E21" s="9">
         <v>18</v>
@@ -2471,16 +2471,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E22" s="9">
         <v>18</v>
@@ -2488,16 +2488,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="9">
         <v>8</v>
@@ -2505,16 +2505,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" s="9">
         <v>8</v>
@@ -2522,13 +2522,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2556,16 +2556,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="9">
         <v>1.5</v>
@@ -2573,13 +2573,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D28">
         <v>0</v>

</xml_diff>